<commit_message>
Fix #253 multiple links and add_cell
</commit_message>
<xml_diff>
--- a/tests/xlsx_data/2.in/case2.xlsx
+++ b/tests/xlsx_data/2.in/case2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Count</t>
   </si>
   <si>
+    <t>RowSum</t>
+  </si>
+  <si>
     <t>c1</t>
   </si>
   <si>
@@ -35,7 +38,7 @@
     <t>c4</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -396,67 +399,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="3">
+        <f>ROUND(SUM(B2), 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="3">
+        <f>ROUND(SUM(B3), 0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="3">
+        <f>ROUND(SUM(B4), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3">
+        <f>ROUND(SUM(B5), 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <f>ROUND(PRODUCT(B2:B5), 0)</f>
         <v>24</v>
       </c>
+      <c r="C6" s="5">
+        <f>ROUND(PRODUCT(C2:C5), 0)</f>
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2 C2 B3 C3 B4 C4 B5 C5 B6 C6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -468,21 +498,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3">
-        <f>ROUND(s1!B6, 0)</f>
+        <f>ROUND('s1'!B6, 0)</f>
         <v>24</v>
       </c>
       <c r="B1" s="2">
-        <f>ROUND(s1!B6, 0)</f>
+        <f>ROUND('s1'!B6, 0)</f>
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1 B1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #253 add features to xlsx for rsaccounting (#254)
* Fix #253 multiple links and add_cell
* allow headers to just be a list
* add_cells handles args more flexibly
* links only need to begin with an alnum
* Allow clearing a default by setting it to None
</commit_message>
<xml_diff>
--- a/tests/xlsx_data/2.in/case2.xlsx
+++ b/tests/xlsx_data/2.in/case2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Count</t>
   </si>
   <si>
+    <t>RowSum</t>
+  </si>
+  <si>
     <t>c1</t>
   </si>
   <si>
@@ -35,7 +38,7 @@
     <t>c4</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -396,67 +399,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="3">
+        <f>ROUND(SUM(B2), 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="3">
+        <f>ROUND(SUM(B3), 0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="3">
+        <f>ROUND(SUM(B4), 0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3">
+        <f>ROUND(SUM(B5), 0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <f>ROUND(PRODUCT(B2:B5), 0)</f>
         <v>24</v>
       </c>
+      <c r="C6" s="5">
+        <f>ROUND(PRODUCT(C2:C5), 0)</f>
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2 C2 B3 C3 B4 C4 B5 C5 B6 C6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -468,21 +498,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3">
-        <f>ROUND(s1!B6, 0)</f>
+        <f>ROUND('s1'!B6, 0)</f>
         <v>24</v>
       </c>
       <c r="B1" s="2">
-        <f>ROUND(s1!B6, 0)</f>
+        <f>ROUND('s1'!B6, 0)</f>
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1 B1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #483 Add IF and MOD (#484)
- percent round_digits adjust fmt digits by 2
- error message format has spurious key
- refactor into _OP_SPECS so can handle adding others
- remove unnecessary space in ROUND()
</commit_message>
<xml_diff>
--- a/tests/xlsx_data/2.in/case2.xlsx
+++ b/tests/xlsx_data/2.in/case2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -23,19 +23,34 @@
     <t>Count</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>RowSum</t>
   </si>
   <si>
     <t>c1</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>c2</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>c3</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>c4</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>Product</t>
@@ -46,9 +61,6 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="@"/>
-    <numFmt numFmtId="164" formatCode="@"/>
-    <numFmt numFmtId="165" formatCode="$#,##0"/>
     <numFmt numFmtId="164" formatCode="@"/>
     <numFmt numFmtId="165" formatCode="$#,##0"/>
   </numFmts>
@@ -399,18 +411,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="2" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,72 +432,88 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <f>ROUND(SUM(B2), 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <f>ROUND(SUM(B2,C2),0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <f>ROUND(SUM(B3,C3),0)</f>
         <v>4</v>
       </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3">
-        <f>ROUND(SUM(B3), 0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
-        <f>ROUND(SUM(B4), 0)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
+        <f>ROUND(SUM(B4,C4),0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
-        <f>ROUND(SUM(B5), 0)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <f>ROUND(SUM(B5,C5),0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5">
-        <f>ROUND(PRODUCT(B2:B5), 0)</f>
+        <f>ROUND(PRODUCT(B2:B5),0)</f>
         <v>24</v>
       </c>
-      <c r="C6" s="5">
-        <f>ROUND(PRODUCT(C2:C5), 0)</f>
-        <v>24</v>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5">
+        <f>ROUND(PRODUCT(D2:D5),0)</f>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2 C2 B3 C3 B4 C4 B5 C5 B6 C6" numberStoredAsText="1"/>
+    <ignoredError sqref="B2 C2 D2 B3 C3 D3 B4 C4 D4 B5 C5 D5 B6 D6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -504,11 +532,11 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3">
-        <f>ROUND('s1'!B6, 0)</f>
+        <f>ROUND('s1'!B6,0)</f>
         <v>24</v>
       </c>
       <c r="B1" s="2">
-        <f>ROUND('s1'!B6, 0)</f>
+        <f>ROUND('s1'!B6,0)</f>
         <v>24</v>
       </c>
     </row>

</xml_diff>